<commit_message>
Corrected schematic for OPAMP connection
</commit_message>
<xml_diff>
--- a/Aimac/1.5KPS/Clist.xlsx
+++ b/Aimac/1.5KPS/Clist.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Powersupply\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Powersupply\PCB\PCB\Aimac\1.5KPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" tabRatio="199"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" tabRatio="199" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="PCB" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>S.No</t>
   </si>
@@ -225,6 +225,30 @@
   </si>
   <si>
     <t>1K ohm, 0.25W, MFR</t>
+  </si>
+  <si>
+    <t>PCB VERSION -1 correction</t>
+  </si>
+  <si>
+    <t>Resistor pad size reduce</t>
+  </si>
+  <si>
+    <t>Resistor pad gap reduce</t>
+  </si>
+  <si>
+    <t>cap pad size to 6mm</t>
+  </si>
+  <si>
+    <t>New CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12V power pin and DIP RMC gap increse </t>
+  </si>
+  <si>
+    <t>NTC pad size increse</t>
+  </si>
+  <si>
+    <t>NTC pad need to redesign( both pin not in stright line)</t>
   </si>
 </sst>
 </file>
@@ -278,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,6 +314,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,19 +670,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E38"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.0546875" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.27734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -670,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -687,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -704,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -721,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -738,7 +767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -755,7 +784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -772,7 +801,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -789,7 +818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -806,7 +835,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -823,7 +852,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -840,7 +869,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -857,7 +886,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -874,7 +903,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
@@ -888,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
@@ -902,7 +931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
@@ -916,7 +945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
@@ -930,7 +959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -944,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -958,7 +987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -972,7 +1001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -986,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -1000,7 +1029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -1014,37 +1043,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>47</v>
       </c>
@@ -1068,14 +1097,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A7:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="8"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1089,7 +1193,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Modified after 1st version up. 1) REplaced with new CT 2) Resistor size and pad size reduced. 3) all disk cap replaced with SMD 4) Removed RESET sWD 5) REmove all POT for VI measurement. 6) Corrected Wrong Connection. 7) Adjusted Poer track as much as bigger.
</commit_message>
<xml_diff>
--- a/Aimac/1.5KPS/Clist.xlsx
+++ b/Aimac/1.5KPS/Clist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>S.No</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>NTC pad need to redesign( both pin not in stright line)</t>
+  </si>
+  <si>
+    <t>Clean copper pour for un connected parts.</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1103,7 @@
   <dimension ref="A7:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1175,6 +1178,9 @@
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>